<commit_message>
fixing tables for part 1
</commit_message>
<xml_diff>
--- a/assignment8/HW8_Tables.xlsx
+++ b/assignment8/HW8_Tables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20408"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jcarv\Downloads\HW8 pt 1 REV\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RENRIQ~1\AppData\Roaming\MobaXterm\slash\RemoteFiles\67244_2_32\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1231A6D2-B9F5-492E-95F1-A2D3BBE0D5BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21B270D0-20F6-4855-8EB6-3DDB00D1C3EF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{3CA6DCAC-A371-4679-AB22-24948FF5CFA8}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="13890" xr2:uid="{3CA6DCAC-A371-4679-AB22-24948FF5CFA8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,23 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="12">
   <si>
     <t>Pure Python</t>
   </si>
@@ -48,9 +37,6 @@
   </si>
   <si>
     <t>Numba2*</t>
-  </si>
-  <si>
-    <t>* = total execution is sum of dummy compile run and real run</t>
   </si>
   <si>
     <t>Jit Decorator</t>
@@ -73,12 +59,15 @@
   <si>
     <t>N/A</t>
   </si>
+  <si>
+    <t>Dummy Execution Time (s)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -93,6 +82,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -130,7 +125,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -141,6 +136,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -263,7 +264,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$K$4:$K$9</c:f>
+              <c:f>Sheet1!$L$4:$L$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -290,7 +291,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$M$4:$M$9</c:f>
+              <c:f>Sheet1!$N$4:$N$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -723,7 +724,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$K$4:$K$8</c:f>
+              <c:f>Sheet1!$L$4:$L$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -747,7 +748,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$N$4:$N$9</c:f>
+              <c:f>Sheet1!$O$4:$O$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -2192,13 +2193,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>17</xdr:row>
       <xdr:rowOff>11430</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
+      <xdr:col>11</xdr:col>
       <xdr:colOff>731520</xdr:colOff>
       <xdr:row>32</xdr:row>
       <xdr:rowOff>11430</xdr:rowOff>
@@ -2228,13 +2229,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
+      <xdr:col>11</xdr:col>
       <xdr:colOff>746760</xdr:colOff>
       <xdr:row>17</xdr:row>
       <xdr:rowOff>11430</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
+      <xdr:col>17</xdr:col>
       <xdr:colOff>373380</xdr:colOff>
       <xdr:row>32</xdr:row>
       <xdr:rowOff>11430</xdr:rowOff>
@@ -2266,9 +2267,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2306,7 +2307,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -2412,7 +2413,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2554,7 +2555,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2562,217 +2563,226 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAC3087F-0F70-4EF8-8066-1D273FA1DBB8}">
-  <dimension ref="A1:N9"/>
+  <dimension ref="A1:O9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1:N9"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.88671875" customWidth="1"/>
-    <col min="2" max="2" width="22.5546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="21.33203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.85546875" customWidth="1"/>
+    <col min="2" max="2" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="21.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>4</v>
-      </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="L1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="N1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="O1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="N1" s="2" t="s">
-        <v>7</v>
-      </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1">
-        <v>12.447417497634801</v>
-      </c>
-      <c r="J2" s="3" t="s">
+      <c r="B2" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="5">
+        <v>12.1664419174194</v>
+      </c>
+      <c r="K2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="K2" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="L2" s="3">
+      <c r="L2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="M2" s="3">
         <v>86.920012</v>
       </c>
-      <c r="M2" s="3" t="s">
-        <v>11</v>
-      </c>
       <c r="N2" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="1">
-        <f>8.7905855178833+0.66768455505371</f>
-        <v>9.4582700729370117</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>5</v>
+      <c r="B3" s="6">
+        <v>0.88648128509521396</v>
+      </c>
+      <c r="C3" s="5">
+        <v>8.3290262222290004</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="L3" s="3">
+        <v>4</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="M3" s="3">
         <f>1.722404</f>
         <v>1.722404</v>
       </c>
-      <c r="M3" s="3" t="s">
-        <v>11</v>
-      </c>
       <c r="N3" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="O3" s="3" t="s">
+        <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="1">
-        <f>0.356932878494262+0.570966482162475</f>
-        <v>0.92789936065673695</v>
-      </c>
-      <c r="J4" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="K4" s="3">
+      <c r="B4" s="6">
+        <v>0.56451439857482899</v>
+      </c>
+      <c r="C4" s="5">
+        <v>0.35559582710266102</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="L4" s="3">
         <v>1</v>
       </c>
-      <c r="L4" s="3">
+      <c r="M4" s="3">
         <v>0.122196</v>
       </c>
-      <c r="M4" s="3">
-        <f>$L$4/L4</f>
+      <c r="N4" s="3">
+        <f>$M$4/M4</f>
         <v>1</v>
       </c>
-      <c r="N4" s="3">
-        <f>M4/1</f>
+      <c r="O4" s="3">
+        <f>N4/1</f>
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="J5" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="K5" s="3">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="K5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="L5" s="3">
         <v>2</v>
       </c>
-      <c r="L5" s="3">
+      <c r="M5" s="3">
         <v>0.11419799999999999</v>
       </c>
-      <c r="M5" s="3">
-        <f t="shared" ref="M5:M9" si="0">$L$4/L5</f>
+      <c r="N5" s="3">
+        <f t="shared" ref="N5:N9" si="0">$M$4/M5</f>
         <v>1.0700362528240426</v>
       </c>
-      <c r="N5" s="3">
-        <f>M5/2</f>
+      <c r="O5" s="3">
+        <f>N5/2</f>
         <v>0.53501812641202129</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="J6" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="K6" s="3">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="K6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="L6" s="3">
         <v>4</v>
       </c>
-      <c r="L6" s="3">
+      <c r="M6" s="3">
         <v>0.12906899999999999</v>
       </c>
-      <c r="M6" s="3">
+      <c r="N6" s="3">
         <f t="shared" si="0"/>
         <v>0.94674941310461858</v>
       </c>
-      <c r="N6" s="3">
-        <f>M6/4</f>
+      <c r="O6" s="3">
+        <f>N6/4</f>
         <v>0.23668735327615464</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="J7" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="K7" s="3">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="K7" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="L7" s="3">
         <v>8</v>
       </c>
-      <c r="L7" s="4">
+      <c r="M7" s="4">
         <v>0.11800099999999999</v>
       </c>
-      <c r="M7" s="3">
+      <c r="N7" s="3">
         <f t="shared" si="0"/>
         <v>1.035550546181812</v>
       </c>
-      <c r="N7" s="3">
-        <f>M7/8</f>
+      <c r="O7" s="3">
+        <f>N7/8</f>
         <v>0.1294438182727265</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="J8" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="K8" s="3">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="K8" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="L8" s="3">
         <v>16</v>
       </c>
-      <c r="L8" s="3">
+      <c r="M8" s="3">
         <v>0.131884</v>
       </c>
-      <c r="M8" s="3">
+      <c r="N8" s="3">
         <f t="shared" si="0"/>
         <v>0.92654150617209063</v>
       </c>
-      <c r="N8" s="3">
-        <f>M8/16</f>
+      <c r="O8" s="3">
+        <f>N8/16</f>
         <v>5.7908844135755665E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="J9" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="K9" s="3">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="K9" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="L9" s="3">
         <v>20</v>
       </c>
-      <c r="L9" s="3">
+      <c r="M9" s="3">
         <v>0.13680200000000001</v>
       </c>
-      <c r="M9" s="3">
+      <c r="N9" s="3">
         <f t="shared" si="0"/>
         <v>0.89323255507960408</v>
       </c>
-      <c r="N9" s="3">
-        <f>M9/20</f>
+      <c r="O9" s="3">
+        <f>N9/20</f>
         <v>4.4661627753980207E-2</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updating word and excel file
</commit_message>
<xml_diff>
--- a/assignment8/HW8_Tables.xlsx
+++ b/assignment8/HW8_Tables.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20408"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jcarv\AppData\Roaming\MobaXterm\slash\RemoteFiles\3743328_2_5\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RENRIQ~1\AppData\Roaming\MobaXterm\slash\RemoteFiles\394710_2_7\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8B99CFC-5EBA-4F69-939C-A3C2052B7318}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D25D0A1-5CB9-49FA-95AC-F33144565401}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{3CA6DCAC-A371-4679-AB22-24948FF5CFA8}"/>
   </bookViews>
@@ -20,23 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="19">
   <si>
     <t>Pure Python</t>
   </si>
@@ -73,12 +62,33 @@
   <si>
     <t>Dummy Execution Time (s)</t>
   </si>
+  <si>
+    <t>3x3</t>
+  </si>
+  <si>
+    <t>10x10</t>
+  </si>
+  <si>
+    <t>100x100</t>
+  </si>
+  <si>
+    <t>1000x1000</t>
+  </si>
+  <si>
+    <t>Cython Execution Time (s)</t>
+  </si>
+  <si>
+    <t>Numpy Execution Time(s)</t>
+  </si>
+  <si>
+    <t>Matrix size</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -97,6 +107,12 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
@@ -136,7 +152,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -150,6 +166,12 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2275,9 +2297,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2315,7 +2337,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -2421,7 +2443,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2563,7 +2585,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2571,24 +2593,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAC3087F-0F70-4EF8-8066-1D273FA1DBB8}">
-  <dimension ref="A1:O9"/>
+  <dimension ref="A1:O11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O15" sqref="O15"/>
+      <selection activeCell="A7" sqref="A7:C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.88671875" customWidth="1"/>
-    <col min="2" max="2" width="24.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.5546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="21.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.85546875" customWidth="1"/>
+    <col min="2" max="2" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="21.28515625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="5" t="s">
         <v>11</v>
@@ -2612,7 +2634,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -2638,7 +2660,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -2665,7 +2687,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -2693,7 +2715,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="K5" s="3" t="s">
         <v>9</v>
       </c>
@@ -2712,7 +2734,7 @@
         <v>0.81335438670935367</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="K6" s="3" t="s">
         <v>9</v>
       </c>
@@ -2731,7 +2753,16 @@
         <v>0.5347343428852106</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>17</v>
+      </c>
       <c r="K7" s="3" t="s">
         <v>9</v>
       </c>
@@ -2750,7 +2781,16 @@
         <v>0.38205500046848778</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="7">
+        <v>3.4332275390625E-5</v>
+      </c>
+      <c r="C8" s="6">
+        <v>2.1492958068847601E-2</v>
+      </c>
       <c r="K8" s="3" t="s">
         <v>9</v>
       </c>
@@ -2769,7 +2809,16 @@
         <v>0.3725928390335968</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="7">
+        <v>3.76701354980468E-5</v>
+      </c>
+      <c r="C9" s="7">
+        <v>3.8623809814453098E-5</v>
+      </c>
       <c r="K9" s="3" t="s">
         <v>9</v>
       </c>
@@ -2786,6 +2835,28 @@
       <c r="O9" s="3">
         <f>N9/20</f>
         <v>0.32091980381143859</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="6">
+        <v>3.2825469970703099E-3</v>
+      </c>
+      <c r="C10" s="6">
+        <v>3.0381679534912099E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="6">
+        <v>1.2439148426055899</v>
+      </c>
+      <c r="C11" s="6">
+        <v>1.36716365814208E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>